<commit_message>
Feat: Complete Phase 9 & 10 (Learning System, Common Rules, UI Overhaul)
- Learning System: Integrated LearningService, added Dashboard, optimized performance.
- Common Rules: Added 'is_common' feature for cross-sheet rule application.
- UI/UX: Refactored sidebar, separated Dashboard tabs, improved Fix UI.
- Fix Logic: Enhanced date pattern detection and auto-fix capabilities.
- Validation: Verified K-IFRS outlier detection and composite rules.
</commit_message>
<xml_diff>
--- a/C.xlsx
+++ b/C.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\kihoon_\by_prompt\gemini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\kihoon_\by_prompt\claude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC6E47-6468-4B89-973D-F67555A29CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE527C5-EA0A-479D-B603-5BF4981BC816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2052" yWindow="744" windowWidth="20988" windowHeight="10788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="규칙 목록" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -678,7 +678,7 @@
   <dimension ref="B2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>

</xml_diff>